<commit_message>
Atualização e adição de documentos
</commit_message>
<xml_diff>
--- a/documentação/GreenSystem - Visão e Backlog.xlsx
+++ b/documentação/GreenSystem - Visão e Backlog.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lidih\Desktop\PROJETO INTER\P I 3 - CIDADES INTELIGENTES\1000 - Documentos\1100 - Visão e Backlog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\broliveirabg\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4D5892-9ACF-4EC3-ACE9-AEC66F0756E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C55B609-2E73-4FB9-8605-518C42634841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{92AD5405-7321-49B6-96B3-B7D17F9632E0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{92AD5405-7321-49B6-96B3-B7D17F9632E0}"/>
   </bookViews>
   <sheets>
     <sheet name="GreenSystem" sheetId="2" r:id="rId1"/>
     <sheet name="Planilha1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">GreenSystem!$A$9:$AV$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">GreenSystem!$A$9:$AW$9</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Planilha1!$A$10:$AV$10</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="112">
   <si>
     <t>Produt Owner</t>
   </si>
@@ -291,9 +291,6 @@
     <t>Com o usuário, anseio por receber notificações via SMS, que proporcionam maior visibilidade e facilidade, informando-me prontamente sobre eventuais problemas relacionados ao consumo de energia que possam ocorrer. Além disso, ter uma página "dicas" será extremamente útil para me informar corretamente sobre boas práticas que posso tomar para reduzir o consumo.</t>
   </si>
   <si>
-    <t>Verificar vasão de água para medição</t>
-  </si>
-  <si>
     <t>Informar área com escassez de água</t>
   </si>
   <si>
@@ -402,6 +399,12 @@
   </si>
   <si>
     <t>Receber notificações via - sms</t>
+  </si>
+  <si>
+    <t>Verificar vazão de água para medição</t>
+  </si>
+  <si>
+    <t>Estimativa de tempo (horas)</t>
   </si>
 </sst>
 </file>
@@ -601,6 +604,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -613,26 +628,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -652,7 +655,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -948,10 +951,621 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38631BF7-F670-4F6C-8E32-580607EFF44C}">
-  <dimension ref="A1:AV47"/>
+  <dimension ref="A1:AW47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F8" zoomScaleNormal="100" zoomScaleSheetLayoutView="98" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="98" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="14.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="41.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="202.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="174.5703125" style="5" customWidth="1"/>
+    <col min="8" max="49" width="9.140625" style="3"/>
+    <col min="50" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:49" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:49" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="6"/>
+      <c r="AA5" s="6"/>
+      <c r="AB5" s="6"/>
+      <c r="AC5" s="6"/>
+      <c r="AD5" s="6"/>
+      <c r="AE5" s="6"/>
+      <c r="AF5" s="6"/>
+      <c r="AG5" s="6"/>
+      <c r="AH5" s="6"/>
+      <c r="AI5" s="6"/>
+      <c r="AJ5" s="6"/>
+      <c r="AK5" s="6"/>
+      <c r="AL5" s="6"/>
+      <c r="AM5" s="6"/>
+      <c r="AN5" s="6"/>
+      <c r="AO5" s="6"/>
+      <c r="AP5" s="6"/>
+      <c r="AQ5" s="6"/>
+      <c r="AR5" s="6"/>
+      <c r="AS5" s="6"/>
+      <c r="AT5" s="6"/>
+      <c r="AU5" s="6"/>
+      <c r="AV5" s="6"/>
+      <c r="AW5" s="6"/>
+    </row>
+    <row r="6" spans="1:49" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+    </row>
+    <row r="7" spans="1:49" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6"/>
+      <c r="B7" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="6"/>
+      <c r="AA7" s="6"/>
+      <c r="AB7" s="6"/>
+      <c r="AC7" s="6"/>
+      <c r="AD7" s="6"/>
+      <c r="AE7" s="6"/>
+      <c r="AF7" s="6"/>
+      <c r="AG7" s="6"/>
+      <c r="AH7" s="6"/>
+      <c r="AI7" s="6"/>
+      <c r="AJ7" s="6"/>
+      <c r="AK7" s="6"/>
+      <c r="AL7" s="6"/>
+      <c r="AM7" s="6"/>
+      <c r="AN7" s="6"/>
+      <c r="AO7" s="6"/>
+      <c r="AP7" s="6"/>
+      <c r="AQ7" s="6"/>
+      <c r="AR7" s="6"/>
+      <c r="AS7" s="6"/>
+      <c r="AT7" s="6"/>
+      <c r="AU7" s="6"/>
+      <c r="AV7" s="6"/>
+      <c r="AW7" s="6"/>
+    </row>
+    <row r="8" spans="1:49" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="15"/>
+    </row>
+    <row r="9" spans="1:49" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
+      <c r="V9" s="8"/>
+      <c r="W9" s="8"/>
+      <c r="X9" s="8"/>
+      <c r="Y9" s="8"/>
+      <c r="Z9" s="8"/>
+      <c r="AA9" s="8"/>
+      <c r="AB9" s="8"/>
+      <c r="AC9" s="8"/>
+      <c r="AD9" s="8"/>
+      <c r="AE9" s="8"/>
+      <c r="AF9" s="8"/>
+      <c r="AG9" s="8"/>
+      <c r="AH9" s="8"/>
+      <c r="AI9" s="8"/>
+      <c r="AJ9" s="8"/>
+      <c r="AK9" s="8"/>
+      <c r="AL9" s="8"/>
+      <c r="AM9" s="8"/>
+      <c r="AN9" s="8"/>
+      <c r="AO9" s="8"/>
+      <c r="AP9" s="8"/>
+      <c r="AQ9" s="8"/>
+      <c r="AR9" s="8"/>
+      <c r="AS9" s="8"/>
+      <c r="AT9" s="8"/>
+      <c r="AU9" s="8"/>
+      <c r="AV9" s="8"/>
+      <c r="AW9" s="8"/>
+    </row>
+    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="B10" s="4">
+        <v>1</v>
+      </c>
+      <c r="C10" s="4">
+        <v>100</v>
+      </c>
+      <c r="D10" s="4">
+        <v>50</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="B11" s="4">
+        <v>2</v>
+      </c>
+      <c r="C11" s="4">
+        <v>90</v>
+      </c>
+      <c r="D11" s="4">
+        <v>35</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="B12" s="4">
+        <v>3</v>
+      </c>
+      <c r="C12" s="4">
+        <v>95</v>
+      </c>
+      <c r="D12" s="4">
+        <v>40</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="B13" s="4">
+        <v>4</v>
+      </c>
+      <c r="C13" s="4">
+        <v>75</v>
+      </c>
+      <c r="D13" s="4">
+        <v>25</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:49" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="4">
+        <v>5</v>
+      </c>
+      <c r="C14" s="4">
+        <v>70</v>
+      </c>
+      <c r="D14" s="4">
+        <v>30</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="B15" s="4">
+        <v>6</v>
+      </c>
+      <c r="C15" s="4">
+        <v>85</v>
+      </c>
+      <c r="D15" s="4">
+        <v>30</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:49" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="4">
+        <v>7</v>
+      </c>
+      <c r="C16" s="4">
+        <v>80</v>
+      </c>
+      <c r="D16" s="4">
+        <v>30</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="4">
+        <v>8</v>
+      </c>
+      <c r="C17" s="4">
+        <v>60</v>
+      </c>
+      <c r="D17" s="4">
+        <v>35</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="4">
+        <v>9</v>
+      </c>
+      <c r="C18" s="4">
+        <v>65</v>
+      </c>
+      <c r="D18" s="4">
+        <v>25</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="4">
+        <v>10</v>
+      </c>
+      <c r="C19" s="4">
+        <v>50</v>
+      </c>
+      <c r="D19" s="4">
+        <v>40</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B20" s="4">
+        <v>11</v>
+      </c>
+      <c r="C20" s="4">
+        <v>55</v>
+      </c>
+      <c r="D20" s="4">
+        <v>35</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="4">
+        <v>12</v>
+      </c>
+      <c r="C21" s="4">
+        <v>40</v>
+      </c>
+      <c r="D21" s="4">
+        <v>35</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="4">
+        <v>13</v>
+      </c>
+      <c r="C22" s="4">
+        <v>30</v>
+      </c>
+      <c r="D22" s="4">
+        <v>30</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B23" s="4">
+        <v>14</v>
+      </c>
+      <c r="C23" s="4">
+        <v>35</v>
+      </c>
+      <c r="D23" s="4">
+        <v>25</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B24" s="4">
+        <v>15</v>
+      </c>
+      <c r="C24" s="4">
+        <v>25</v>
+      </c>
+      <c r="D24" s="4">
+        <v>40</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B25" s="4">
+        <v>16</v>
+      </c>
+      <c r="C25" s="4">
+        <v>45</v>
+      </c>
+      <c r="D25" s="4">
+        <v>45</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:7" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:7" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="2:7" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:7" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="2:7" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:7" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <autoFilter ref="A9:AW9" xr:uid="{C93F1059-8B86-4942-9620-E8C88DC98ADD}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A10:AW25">
+      <sortCondition descending="1" ref="C9"/>
+    </sortState>
+  </autoFilter>
+  <mergeCells count="7">
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C93F1059-8B86-4942-9620-E8C88DC98ADD}">
+  <dimension ref="A1:AV51"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="98" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,7 +1575,7 @@
     <col min="3" max="3" width="10.140625" style="5" customWidth="1"/>
     <col min="4" max="4" width="41.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="202.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="174.5703125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="139.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="48" width="9.140625" style="3"/>
     <col min="49" max="16384" width="9.140625" style="5"/>
   </cols>
@@ -971,10 +1585,10 @@
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="D2" s="12"/>
+      <c r="C2" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="16"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
@@ -982,10 +1596,10 @@
       <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="D3" s="12"/>
+      <c r="C3" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="16"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
@@ -993,22 +1607,22 @@
       <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="15"/>
+      <c r="C4" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="18"/>
+      <c r="E4" s="19"/>
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:48" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -1053,23 +1667,23 @@
       <c r="AV5" s="6"/>
     </row>
     <row r="6" spans="1:48" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-    </row>
-    <row r="7" spans="1:48" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+    </row>
+    <row r="7" spans="1:48" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -1113,576 +1727,23 @@
       <c r="AU7" s="6"/>
       <c r="AV7" s="6"/>
     </row>
-    <row r="8" spans="1:48" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="21"/>
-    </row>
-    <row r="9" spans="1:48" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="8"/>
-      <c r="S9" s="8"/>
-      <c r="T9" s="8"/>
-      <c r="U9" s="8"/>
-      <c r="V9" s="8"/>
-      <c r="W9" s="8"/>
-      <c r="X9" s="8"/>
-      <c r="Y9" s="8"/>
-      <c r="Z9" s="8"/>
-      <c r="AA9" s="8"/>
-      <c r="AB9" s="8"/>
-      <c r="AC9" s="8"/>
-      <c r="AD9" s="8"/>
-      <c r="AE9" s="8"/>
-      <c r="AF9" s="8"/>
-      <c r="AG9" s="8"/>
-      <c r="AH9" s="8"/>
-      <c r="AI9" s="8"/>
-      <c r="AJ9" s="8"/>
-      <c r="AK9" s="8"/>
-      <c r="AL9" s="8"/>
-      <c r="AM9" s="8"/>
-      <c r="AN9" s="8"/>
-      <c r="AO9" s="8"/>
-      <c r="AP9" s="8"/>
-      <c r="AQ9" s="8"/>
-      <c r="AR9" s="8"/>
-      <c r="AS9" s="8"/>
-      <c r="AT9" s="8"/>
-      <c r="AU9" s="8"/>
-      <c r="AV9" s="8"/>
-    </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="B10" s="4">
-        <v>1</v>
-      </c>
-      <c r="C10" s="4">
-        <v>100</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="B11" s="4">
-        <v>2</v>
-      </c>
-      <c r="C11" s="4">
-        <v>90</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="B12" s="4">
-        <v>3</v>
-      </c>
-      <c r="C12" s="4">
-        <v>85</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="B13" s="4">
-        <v>4</v>
-      </c>
-      <c r="C13" s="4">
-        <v>80</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="14" spans="1:48" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="4">
+    <row r="8" spans="1:48" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+    </row>
+    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="B9" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="4">
-        <v>80</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="B15" s="4">
-        <v>6</v>
-      </c>
-      <c r="C15" s="4">
-        <v>70</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="16" spans="1:48" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="4">
-        <v>7</v>
-      </c>
-      <c r="C16" s="4">
-        <v>65</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="4">
-        <v>8</v>
-      </c>
-      <c r="C17" s="4">
-        <v>55</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="4">
-        <v>9</v>
-      </c>
-      <c r="C18" s="4">
-        <v>50</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="4">
-        <v>10</v>
-      </c>
-      <c r="C19" s="4">
-        <v>45</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B20" s="4">
-        <v>11</v>
-      </c>
-      <c r="C20" s="4">
-        <v>40</v>
-      </c>
-      <c r="D20" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="4">
-        <v>12</v>
-      </c>
-      <c r="C21" s="4">
-        <v>35</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="4">
-        <v>13</v>
-      </c>
-      <c r="C22" s="4">
-        <v>30</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B23" s="4">
-        <v>14</v>
-      </c>
-      <c r="C23" s="4">
-        <v>25</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B24" s="4">
-        <v>15</v>
-      </c>
-      <c r="C24" s="4">
-        <v>20</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B25" s="4">
-        <v>16</v>
-      </c>
-      <c r="C25" s="4">
-        <v>15</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <autoFilter ref="A9:AV9" xr:uid="{C93F1059-8B86-4942-9620-E8C88DC98ADD}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A10:AV25">
-      <sortCondition descending="1" ref="C9"/>
-    </sortState>
-  </autoFilter>
-  <mergeCells count="7">
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B7:F7"/>
-  </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C93F1059-8B86-4942-9620-E8C88DC98ADD}">
-  <dimension ref="A1:AV51"/>
-  <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="98" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="2" width="14.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="41.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="202.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="139.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="48" width="9.140625" style="3"/>
-    <col min="49" max="16384" width="9.140625" style="5"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:48" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:48" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
-      <c r="S5" s="6"/>
-      <c r="T5" s="6"/>
-      <c r="U5" s="6"/>
-      <c r="V5" s="6"/>
-      <c r="W5" s="6"/>
-      <c r="X5" s="6"/>
-      <c r="Y5" s="6"/>
-      <c r="Z5" s="6"/>
-      <c r="AA5" s="6"/>
-      <c r="AB5" s="6"/>
-      <c r="AC5" s="6"/>
-      <c r="AD5" s="6"/>
-      <c r="AE5" s="6"/>
-      <c r="AF5" s="6"/>
-      <c r="AG5" s="6"/>
-      <c r="AH5" s="6"/>
-      <c r="AI5" s="6"/>
-      <c r="AJ5" s="6"/>
-      <c r="AK5" s="6"/>
-      <c r="AL5" s="6"/>
-      <c r="AM5" s="6"/>
-      <c r="AN5" s="6"/>
-      <c r="AO5" s="6"/>
-      <c r="AP5" s="6"/>
-      <c r="AQ5" s="6"/>
-      <c r="AR5" s="6"/>
-      <c r="AS5" s="6"/>
-      <c r="AT5" s="6"/>
-      <c r="AU5" s="6"/>
-      <c r="AV5" s="6"/>
-    </row>
-    <row r="6" spans="1:48" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-    </row>
-    <row r="7" spans="1:48" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="6"/>
-      <c r="S7" s="6"/>
-      <c r="T7" s="6"/>
-      <c r="U7" s="6"/>
-      <c r="V7" s="6"/>
-      <c r="W7" s="6"/>
-      <c r="X7" s="6"/>
-      <c r="Y7" s="6"/>
-      <c r="Z7" s="6"/>
-      <c r="AA7" s="6"/>
-      <c r="AB7" s="6"/>
-      <c r="AC7" s="6"/>
-      <c r="AD7" s="6"/>
-      <c r="AE7" s="6"/>
-      <c r="AF7" s="6"/>
-      <c r="AG7" s="6"/>
-      <c r="AH7" s="6"/>
-      <c r="AI7" s="6"/>
-      <c r="AJ7" s="6"/>
-      <c r="AK7" s="6"/>
-      <c r="AL7" s="6"/>
-      <c r="AM7" s="6"/>
-      <c r="AN7" s="6"/>
-      <c r="AO7" s="6"/>
-      <c r="AP7" s="6"/>
-      <c r="AQ7" s="6"/>
-      <c r="AR7" s="6"/>
-      <c r="AS7" s="6"/>
-      <c r="AT7" s="6"/>
-      <c r="AU7" s="6"/>
-      <c r="AV7" s="6"/>
-    </row>
-    <row r="8" spans="1:48" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-    </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="B9" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
     </row>
     <row r="10" spans="1:48" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>

</xml_diff>

<commit_message>
Atualização do arquivo de backlog
</commit_message>
<xml_diff>
--- a/documentação/GreenSystem - Visão e Backlog.xlsx
+++ b/documentação/GreenSystem - Visão e Backlog.xlsx
@@ -20,24 +20,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t xml:space="preserve">Produt Owner</t>
   </si>
   <si>
-    <t>Município</t>
-  </si>
-  <si>
     <t xml:space="preserve">Scrum Master</t>
   </si>
   <si>
-    <t xml:space="preserve">Vinícius Tiberio</t>
-  </si>
-  <si>
     <t>Time</t>
   </si>
   <si>
-    <t xml:space="preserve">Lidiane Marques, Micaella Oliveira, Mikelly Oliveira, Luan Rocha</t>
+    <t xml:space="preserve">Lidiane Marques, Micaella Oliveira, Mikelly Oliveira, Luan Rocha, Vinicius Tibério, José Victor</t>
   </si>
   <si>
     <t xml:space="preserve">Nome do Aplicativo</t>
@@ -74,19 +68,19 @@
     <t xml:space="preserve">Verificar vazão de água para medição</t>
   </si>
   <si>
-    <t xml:space="preserve">Como usuário, gostaria que fosse realizado uma medição da vasão de água para gerar dados que posteriormente possam  me ajudar a economizar.</t>
+    <t xml:space="preserve">Como usuário, gostaria que fosse realizado uma medição da vasão de água para gerar dados que posteriormente possam me ajudar a economizar.</t>
   </si>
   <si>
     <t xml:space="preserve">O sistema deve utilizar os dados presentes coletados nos sensores gerarando uma medição diária do consumo realizado em determinados períodos de tempo.</t>
   </si>
   <si>
-    <t xml:space="preserve">Gerar gráficos de água</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Como usuário, gostaria de visualizar de forma gráfica e intuitiva  a medição de água.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O sistema deve utilizar as medições geradas para criar gráfico visual com os dados de consumo municipal e individual.</t>
+    <t xml:space="preserve">Gerar gráficos de água e energia </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Como usuário, gostaria de visualizar de forma gráfica e intuitiva a medição de água e consumo de energia.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema deve utilizar as medições geradas para criar gráfico visual com os dados de consumo individual.</t>
   </si>
   <si>
     <t xml:space="preserve">Atualizar em tempo real</t>
@@ -101,7 +95,7 @@
     <t xml:space="preserve">Realizar Login</t>
   </si>
   <si>
-    <t xml:space="preserve">Como usuário, gostaria de realizar o login para acessar no meu perfil e ver minhas informações de forma simples e seguras.</t>
+    <t xml:space="preserve">Como usuário e administrador, gostaria de realizar o login para acessar no meu perfil e ver minhas informações de forma simples e seguras.</t>
   </si>
   <si>
     <t xml:space="preserve">Acessar sistema, preencher campo de login, senha e clicar no botão "Entrar".</t>
@@ -117,15 +111,6 @@
 Os clientes recebem e-mails de notificação após o registro com sucesso.</t>
   </si>
   <si>
-    <t xml:space="preserve">Visualizar dados gerais</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Como usuário, gostaria de ter acesso fácil aos dados gerais de meu município para me manter alinhado com o consumo e gastos e comparar com o  geral da cidade para melhor tomada de decisões.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acessar sistema, entrar na página de Dashboard e visualizar gráficos atualizados em tempo real.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Visualizar dados individuais</t>
   </si>
   <si>
@@ -138,76 +123,49 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t xml:space="preserve">Gerar relatórios de consumo de água</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Como usuário,  quero ter o documento em PDF de todas as entradas e saídas de água e gastos para ter a função de documento e apresentar para autoridades municipais, caso necessário.</t>
+    <t xml:space="preserve">Gerar relatórios de consumo de água e energia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Como usuário,  quero ter o documento em PDF de todo o consumo de energia,  entradas e saídas de água e  gastos para ter a função de documento e apresentar para autoridades municipais, caso necessário.</t>
   </si>
   <si>
     <t xml:space="preserve">O sistema deve utilizar os dados coletados para gerar relatórios com períodos de 1, 3, 6  e 12 meses.</t>
   </si>
   <si>
-    <t xml:space="preserve">Comparar consumo de água</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Como usuário, quero realizar uma comparação entre o meu consumo e o do município e que o site gere uma comparação de meu consumo mensal.</t>
+    <t xml:space="preserve">Comparar consumo de água e energia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Como usuário, quero realizar uma comparação entre o meu consumo de energia e água e  que o site gere uma comparação de meu consumo mensal.</t>
   </si>
   <si>
     <t xml:space="preserve">O sistema deve utilizar os dados coletados para realizar a comparação de consumo mês a mês e retornar para o usuário os valores encontrados.</t>
   </si>
   <si>
-    <t xml:space="preserve">Informar área com escassez de água</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Como usuário, quero ter uma visão macro de meu município e visualizar áreas que estão com escassez de água.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O sistema deve utilizar os dados coletados para destacar as áreas que estão com escassez de água e mostrá-las para o usuário em um mapa.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Receber notificações via - sms</t>
   </si>
   <si>
     <t xml:space="preserve">Como usuário, quero receber notificações via SMS (maior visibilidade e facilidade) sobre eventuais problemas que venham a acontecer para me antecipar com possíveis soluções. </t>
   </si>
   <si>
-    <t xml:space="preserve">O sistema irá, automaticamente, gerar uma mesagem de texto e enviar para o usuário um SMS para o número que ele cadastrou.  A mensagem será gerada se algum problema for emcontrado, como: aumento incomum/rápido consumo de água ou energia, tanto individual, quanto municipal. Caso o usuário queira, ele pode rejeitar o recebimento dessas notificações.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gerar gráficos de energia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Com o usuário, gostaria que esses dados passassem por um tratamento e fossem transformados em gráficos intuitivos da medição de energia.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Através da análise dos dados, o site irá mostrar para o usuário, um gráfico de consumo de energia em tempo real. Haverá no menu de navegação, onde existirá o item "Gráficos".</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gerar relatórios de consumo de energia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Com o usuário, solicito ter um documento em PDF que registre todas as entradas e saídas de energia e despesas, a fim de usá-lo como referência e apresentá-lo às autoridades municipais, quando necessário.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O sistema disponibilizará um botão para converter os dados  de consumo de energia mostrados para o usuário em documento PDF.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comparar consumo de energia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Com o usuário, desejo efetuar uma comparação entre meu consumo e o consumo do município, e quero que o site gere uma análise mensal do meu consumo energético. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">O sistema realizará uma comparação entre o consumo de energia diário do usuário e o consumo diário do munícipio. Essa comparação será mostrada através de gráficos e uma mensagem aparacerá para o usuário de acordo com o resultado gerado pelo gráfico. Exemplo: o gráfico mostrou que o consumo de energia do usuário foi maior do que o município, logo, uma mensagem "Consumo alto! Sua casa está gastando mais energia do que a média geral do município. Tente fazer isso para reduzir o consumo."</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Informar área com escassez de energia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Como  usuário, pretendo obter uma visão ampla de meu município e visualizar áreas com escassez de energia. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">O sistema será capaz através da análise de dados coletados, destacar uma área de falta de energia no mapa da cidade do usuário. Isso também estará em uma página dedicada em um botão da barra de navegação e aparecerá junto com a área destacada de escassez de água.</t>
+    <t xml:space="preserve">O sistema irá, automaticamente, gerar uma mesagem de texto e enviar para o usuário um SMS para o número que ele cadastrou.  A mensagem será gerada se algum problema for emcontrado, como: aumento incomum/rápido consumo de água ou energia, Caso o usuário queira, ele pode rejeitar o recebimento dessas notificações.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vizualizar informações dos clientes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Como administrador, consigo vizualizar de forma organizada os nomes, endereços e status do sistema.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema irá mostrar em tela os endereços, nomes e status do sistema dos clientes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vizualizar em mapa os pontos de instalação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Como administrador, posso vizualizar em mapa os pontos de instalação dos clientes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema irá mostrar em tela um mapa do município com os pontos instalados dos clientes.</t>
   </si>
   <si>
     <t xml:space="preserve">Propor soluções para economia</t>
@@ -244,7 +202,6 @@
     </font>
     <font>
       <sz val="11.000000"/>
-      <color indexed="64"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -366,7 +323,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -418,6 +375,12 @@
     </xf>
     <xf fontId="3" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -938,7 +901,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="G11" zoomScale="100" workbookViewId="0">
       <selection activeCell="B8" activeCellId="0" sqref="B8:G8"/>
     </sheetView>
   </sheetViews>
@@ -947,8 +910,8 @@
     <col min="1" max="1" style="2" width="9.140625"/>
     <col bestFit="1" customWidth="1" min="2" max="2" style="1" width="14.28515625"/>
     <col customWidth="1" min="3" max="4" style="1" width="10.140625"/>
-    <col bestFit="1" customWidth="1" min="5" max="5" style="1" width="41.5703125"/>
-    <col bestFit="1" customWidth="1" min="6" max="6" style="1" width="202.85546875"/>
+    <col bestFit="1" customWidth="1" min="5" max="5" style="1" width="53.140625"/>
+    <col customWidth="1" min="6" max="6" style="1" width="184.421875"/>
     <col customWidth="1" min="7" max="7" style="1" width="174.5703125"/>
     <col min="8" max="49" style="2" width="9.140625"/>
     <col min="50" max="16384" style="1" width="9.140625"/>
@@ -959,9 +922,7 @@
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -969,11 +930,9 @@
     </row>
     <row r="3">
       <c r="B3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>3</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -981,10 +940,10 @@
     </row>
     <row r="4">
       <c r="B4" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -994,7 +953,7 @@
     <row r="5" s="7" customFormat="1">
       <c r="A5" s="8"/>
       <c r="B5" s="9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -1046,7 +1005,7 @@
     </row>
     <row r="6" s="2" customFormat="1">
       <c r="B6" s="10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
@@ -1057,7 +1016,7 @@
     <row r="7" s="7" customFormat="1" ht="15.75">
       <c r="A7" s="8"/>
       <c r="B7" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
@@ -1109,7 +1068,7 @@
     </row>
     <row r="8" ht="51.75" customHeight="1">
       <c r="B8" s="11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
@@ -1120,22 +1079,22 @@
     <row r="9" s="14" customFormat="1" ht="42.75">
       <c r="A9" s="15"/>
       <c r="B9" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="E9" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="F9" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="G9" s="16" t="s">
         <v>13</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="16" t="s">
-        <v>15</v>
       </c>
       <c r="H9" s="15"/>
       <c r="I9" s="15"/>
@@ -1191,13 +1150,13 @@
         <v>50</v>
       </c>
       <c r="E10" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="19" t="s">
         <v>16</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="18" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11">
@@ -1211,13 +1170,13 @@
         <v>35</v>
       </c>
       <c r="E11" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="20" t="s">
         <v>19</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" s="18" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="12">
@@ -1231,13 +1190,13 @@
         <v>40</v>
       </c>
       <c r="E12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="19" t="s">
         <v>22</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="18" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="13">
@@ -1251,13 +1210,13 @@
         <v>25</v>
       </c>
       <c r="E13" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="19" t="s">
         <v>25</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G13" s="18" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="14" ht="28.5">
@@ -1270,34 +1229,37 @@
       <c r="D14" s="3">
         <v>30</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G14" s="18" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15">
+    </row>
+    <row r="15" s="2" customFormat="1">
       <c r="B15" s="3">
         <v>6</v>
       </c>
       <c r="C15" s="3">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D15" s="3">
         <v>30</v>
       </c>
       <c r="E15" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="H15" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="G15" s="18" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="16" s="2" customFormat="1">
@@ -1305,22 +1267,19 @@
         <v>7</v>
       </c>
       <c r="C16" s="3">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="D16" s="3">
-        <v>30</v>
-      </c>
-      <c r="E16" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="G16" s="19" t="s">
         <v>35</v>
-      </c>
-      <c r="G16" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="17" s="2" customFormat="1">
@@ -1328,39 +1287,39 @@
         <v>8</v>
       </c>
       <c r="C17" s="3">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D17" s="3">
-        <v>35</v>
-      </c>
-      <c r="E17" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G17" s="18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" s="2" customFormat="1">
+    </row>
+    <row r="18" s="2" customFormat="1" ht="28.5">
       <c r="B18" s="3">
         <v>9</v>
       </c>
       <c r="C18" s="3">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="D18" s="3">
-        <v>25</v>
-      </c>
-      <c r="E18" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18" s="20" t="s">
         <v>41</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G18" s="18" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="19" s="2" customFormat="1">
@@ -1371,19 +1330,19 @@
         <v>50</v>
       </c>
       <c r="D19" s="3">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="E19" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="G19" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G19" s="18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" s="2" customFormat="1" ht="28.5">
+    </row>
+    <row r="20" s="2" customFormat="1" ht="42.75">
       <c r="B20" s="3">
         <v>11</v>
       </c>
@@ -1391,118 +1350,63 @@
         <v>55</v>
       </c>
       <c r="D20" s="3">
-        <v>35</v>
-      </c>
-      <c r="E20" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G20" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="F20" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G20" s="18" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" s="2" customFormat="1">
+    </row>
+    <row r="21" s="2" customFormat="1" ht="28.5">
       <c r="B21" s="3">
         <v>12</v>
       </c>
       <c r="C21" s="3">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D21" s="3">
-        <v>35</v>
-      </c>
-      <c r="E21" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="G21" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="F21" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G21" s="18" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="22" s="2" customFormat="1">
-      <c r="B22" s="3">
-        <v>13</v>
-      </c>
-      <c r="C22" s="3">
-        <v>30</v>
-      </c>
-      <c r="D22" s="3">
-        <v>30</v>
-      </c>
-      <c r="E22" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G22" s="18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" s="2" customFormat="1" ht="42.75">
-      <c r="B23" s="3">
-        <v>14</v>
-      </c>
-      <c r="C23" s="3">
-        <v>35</v>
-      </c>
-      <c r="D23" s="3">
-        <v>25</v>
-      </c>
-      <c r="E23" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="G23" s="18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="24" s="2" customFormat="1" ht="28.5">
-      <c r="B24" s="3">
-        <v>15</v>
-      </c>
-      <c r="C24" s="3">
-        <v>25</v>
-      </c>
-      <c r="D24" s="3">
-        <v>40</v>
-      </c>
-      <c r="E24" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G24" s="18" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" s="2" customFormat="1" ht="28.5">
-      <c r="B25" s="3">
-        <v>16</v>
-      </c>
-      <c r="C25" s="3">
-        <v>45</v>
-      </c>
-      <c r="D25" s="3">
-        <v>45</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F25" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="G25" s="18" t="s">
-        <v>64</v>
-      </c>
-    </row>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" s="2" customFormat="1">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" s="2" customFormat="1">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" s="2" customFormat="1"/>
     <row r="26" s="2" customFormat="1"/>
     <row r="27" s="2" customFormat="1"/>
     <row r="28" s="2" customFormat="1"/>
@@ -1521,10 +1425,6 @@
     <row r="41" s="2" customFormat="1"/>
     <row r="42" s="2" customFormat="1"/>
     <row r="43" s="2" customFormat="1"/>
-    <row r="44" s="2" customFormat="1"/>
-    <row r="45" s="2" customFormat="1"/>
-    <row r="46" s="2" customFormat="1"/>
-    <row r="47" s="2" customFormat="1"/>
   </sheetData>
   <autoFilter ref="A9:AW9">
     <sortState ref="A10:AW25">
@@ -1541,7 +1441,7 @@
     <mergeCell ref="B8:G8"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157500000008" bottom="0.78740157500000008" header="0.31496062000000008" footer="0.31496062000000008"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157500000008" bottom="0.78740157500000008" header="0.31496062000000014" footer="0.31496062000000014"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>

</xml_diff>